<commit_message>
commiting files to depricate repo
</commit_message>
<xml_diff>
--- a/Wakanda_intf_selectors.xlsx
+++ b/Wakanda_intf_selectors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\tyscott\iac\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tyscott\scotttyso\iac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E9AE899-0A65-4365-A671-2148060D5314}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19361DEC-9D64-4B0E-8483-F8BC9684B9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="803" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="115080" yWindow="15990" windowWidth="29040" windowHeight="15360" tabRatio="803" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wakanda-spine101" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="155">
   <si>
     <t>wakanda-spine101 Interface Selectors</t>
   </si>
@@ -500,6 +500,9 @@
   </si>
   <si>
     <t>trunkPort</t>
+  </si>
+  <si>
+    <t>1-4094</t>
   </si>
 </sst>
 </file>
@@ -673,18 +676,18 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="6">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="2" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="2" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1039,40 +1042,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
     </row>
     <row r="2" spans="1:14" ht="17" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
-      <c r="B2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
+      <c r="B2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
     </row>
     <row r="3" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
@@ -2121,40 +2124,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
     </row>
     <row r="2" spans="1:14" ht="17" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
-      <c r="B2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
+      <c r="B2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
     </row>
     <row r="3" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
@@ -3185,8 +3188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54:G55"/>
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="N52" sqref="N52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3203,40 +3206,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
     </row>
     <row r="2" spans="1:14" ht="17" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
-      <c r="B2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
+      <c r="B2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
     </row>
     <row r="3" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
@@ -4664,7 +4667,9 @@
         <v>143</v>
       </c>
       <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
+      <c r="N52" s="9" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="53" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
@@ -4725,7 +4730,7 @@
       <c r="F54" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="G54" s="12" t="s">
+      <c r="G54" s="9" t="s">
         <v>153</v>
       </c>
       <c r="H54" s="1" t="s">
@@ -4765,7 +4770,7 @@
       <c r="F55" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="G55" s="13" t="s">
+      <c r="G55" s="10" t="s">
         <v>153</v>
       </c>
       <c r="H55" s="2" t="s">
@@ -4881,40 +4886,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
     </row>
     <row r="2" spans="1:14" ht="17" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
-      <c r="B2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
+      <c r="B2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
@@ -6403,7 +6408,7 @@
       <c r="F54" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="G54" s="12" t="s">
+      <c r="G54" s="9" t="s">
         <v>153</v>
       </c>
       <c r="H54" s="1" t="s">
@@ -6443,7 +6448,7 @@
       <c r="F55" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="G55" s="13" t="s">
+      <c r="G55" s="10" t="s">
         <v>153</v>
       </c>
       <c r="H55" s="2" t="s">

</xml_diff>